<commit_message>
fixed recent review errors
</commit_message>
<xml_diff>
--- a/customer/Cherry_Customer_Cart.xlsx
+++ b/customer/Cherry_Customer_Cart.xlsx
@@ -107,9 +107,6 @@
     <t>Buy Now Btn</t>
   </si>
   <si>
-    <t>When customer click back arrow btn beside 'YOUR CART' title,  customer will be deliverd to this address  "http://127.0.0.1:8000/".</t>
-  </si>
-  <si>
     <t>item</t>
   </si>
   <si>
@@ -148,10 +145,6 @@
   </si>
   <si>
     <t>cancel btn of each item</t>
-  </si>
-  <si>
-    <t>When customer click 'Delivery' Btn , customer will be deliverd to this address  
-"http://127.0.0.1:8000/deliveryInfo".</t>
   </si>
   <si>
     <t>The grand total costs will be shown in this grand total input box.</t>
@@ -169,14 +162,8 @@
     <t>The total amount of items will be shown in this original total input box.</t>
   </si>
   <si>
-    <t>When customer click Shopping Cart icon from header, customer will be deliverd to this address  "http://127.0.0.1:8000/cart".</t>
-  </si>
-  <si>
     <t xml:space="preserve">When customer did not buy any food from the product page, there is no item in cart and need to click 'Buy Now' btn  for buying foods.
       </t>
-  </si>
-  <si>
-    <t>When customer click 'Buy Now' btn,  customer will be deliverd to this address  "http://127.0.0.1:8000/" to buy more foods.</t>
   </si>
   <si>
     <t>If customer already bought foods, the items will be shown in cart.
@@ -203,6 +190,19 @@
   </si>
   <si>
     <t>2022/03/08</t>
+  </si>
+  <si>
+    <t>When customer click Shopping Cart icon from header, customer will be deliverd to this address  "http://www.website.com/cart".</t>
+  </si>
+  <si>
+    <t>When customer click back arrow btn beside 'YOUR CART' title,  customer will be deliverd to this address  "http://www.website.com/".</t>
+  </si>
+  <si>
+    <t>When customer click 'Buy Now' btn,  customer will be deliverd to this address  "http://www.website.com/" to buy more foods.</t>
+  </si>
+  <si>
+    <t>When customer click 'Delivery' Btn , customer will be deliverd to this address  
+"http://www.website.com/deliveryInfo".</t>
   </si>
 </sst>
 </file>
@@ -254,7 +254,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -575,59 +575,60 @@
     <xf numFmtId="14" fontId="2" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -693,7 +694,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1028,190 +1028,190 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-    </row>
-    <row r="2" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="31" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+    </row>
+    <row r="2" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="36" t="s">
+      <c r="B2" s="33"/>
+      <c r="C2" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="P2" s="37">
+      <c r="P2" s="38">
         <v>44501</v>
       </c>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="53" t="s">
+      <c r="Q2" s="39"/>
+      <c r="R2" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="39" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="40"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="45" t="s">
+    <row r="3" spans="1:18" s="40" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="45"/>
+      <c r="O3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="P3" s="46">
+      <c r="P3" s="47">
         <v>44501</v>
       </c>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="53" t="s">
+      <c r="Q3" s="48"/>
+      <c r="R3" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="53" t="s">
+      <c r="A4" s="28"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="48" t="s">
+    <row r="5" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49" t="s">
+      <c r="C5" s="50"/>
+      <c r="D5" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="50" t="s">
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="50" t="s">
+      <c r="N5" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="O5" s="50" t="s">
+      <c r="O5" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="P5" s="50" t="s">
+      <c r="P5" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="Q5" s="51" t="s">
+      <c r="Q5" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="R5" s="53"/>
-    </row>
-    <row r="6" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="52"/>
-      <c r="B6" s="49" t="s">
+      <c r="R5" s="13"/>
+    </row>
+    <row r="6" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="53"/>
+      <c r="B6" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49" t="s">
+      <c r="C6" s="50"/>
+      <c r="D6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="50" t="s">
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="50" t="s">
+      <c r="N6" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="O6" s="50" t="s">
+      <c r="O6" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="P6" s="50" t="s">
+      <c r="P6" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="Q6" s="51" t="s">
+      <c r="Q6" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="R6" s="53"/>
+      <c r="R6" s="13"/>
     </row>
     <row r="7" spans="1:18" ht="52.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="8">
         <v>1</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="23"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="18"/>
       <c r="M7" s="2" t="s">
         <v>21</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
@@ -1221,26 +1221,26 @@
       <c r="A8" s="8">
         <v>2</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="23"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="18"/>
       <c r="M8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="N8" s="12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
@@ -1250,26 +1250,26 @@
       <c r="A9" s="7">
         <v>3</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
       <c r="M9" s="11" t="s">
         <v>21</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
@@ -1279,26 +1279,26 @@
       <c r="A10" s="7">
         <v>4</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
       <c r="M10" s="11" t="s">
         <v>21</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
@@ -1308,26 +1308,26 @@
       <c r="A11" s="7">
         <v>5</v>
       </c>
-      <c r="B11" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="28"/>
+      <c r="B11" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="23"/>
       <c r="M11" s="11" t="s">
         <v>21</v>
       </c>
       <c r="N11" s="12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
@@ -1337,26 +1337,26 @@
       <c r="A12" s="7">
         <v>6</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="26"/>
+      <c r="D12" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
       <c r="M12" s="11" t="s">
         <v>21</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
@@ -1366,26 +1366,26 @@
       <c r="A13" s="7">
         <v>7</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="26"/>
+      <c r="D13" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
       <c r="M13" s="11" t="s">
         <v>21</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
@@ -1395,26 +1395,26 @@
       <c r="A14" s="7">
         <v>8</v>
       </c>
-      <c r="B14" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
+      <c r="B14" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="26"/>
+      <c r="D14" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
       <c r="M14" s="11" t="s">
         <v>21</v>
       </c>
       <c r="N14" s="12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
@@ -1424,26 +1424,26 @@
       <c r="A15" s="7">
         <v>9</v>
       </c>
-      <c r="B15" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
+      <c r="B15" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="26"/>
+      <c r="D15" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
       <c r="M15" s="11" t="s">
         <v>21</v>
       </c>
       <c r="N15" s="12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
@@ -1453,26 +1453,26 @@
       <c r="A16" s="7">
         <v>10</v>
       </c>
-      <c r="B16" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
+      <c r="B16" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="26"/>
+      <c r="D16" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
       <c r="M16" s="11" t="s">
         <v>21</v>
       </c>
       <c r="N16" s="12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
@@ -1482,26 +1482,26 @@
       <c r="A17" s="7">
         <v>11</v>
       </c>
-      <c r="B17" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
+      <c r="B17" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="26"/>
+      <c r="D17" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
       <c r="M17" s="11" t="s">
         <v>21</v>
       </c>
       <c r="N17" s="12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
@@ -1511,26 +1511,26 @@
       <c r="A18" s="7">
         <v>12</v>
       </c>
-      <c r="B18" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
+      <c r="B18" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="26"/>
+      <c r="D18" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
       <c r="M18" s="11" t="s">
         <v>21</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
@@ -1540,26 +1540,26 @@
       <c r="A19" s="7">
         <v>13</v>
       </c>
-      <c r="B19" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
+      <c r="B19" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="26"/>
+      <c r="D19" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
       <c r="M19" s="11" t="s">
         <v>21</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
@@ -1569,26 +1569,26 @@
       <c r="A20" s="7">
         <v>14</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
+      <c r="B20" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="26"/>
+      <c r="D20" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
       <c r="M20" s="11" t="s">
         <v>21</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
@@ -1618,21 +1618,15 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:L8"/>
-    <mergeCell ref="D14:L14"/>
-    <mergeCell ref="D11:L11"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:L9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:L10"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:L15"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D12:L12"/>
-    <mergeCell ref="D13:L13"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:L5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:L6"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="C2:N3"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="A4:Q4"/>
@@ -1649,15 +1643,21 @@
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:L1"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:L5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:L6"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="C2:N3"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:L15"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D12:L12"/>
+    <mergeCell ref="D13:L13"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:L8"/>
+    <mergeCell ref="D14:L14"/>
+    <mergeCell ref="D11:L11"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:L9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="41" orientation="portrait" horizontalDpi="300" verticalDpi="1200" r:id="rId1"/>

</xml_diff>